<commit_message>
updates from 3/12 to 3/21
updates to the following controls
V-2236
V-2242
V-2243
V-2246
V-2247
V-2248
V-2256
V-2257
V-2259
V-6485
V-6577
V-13613
V-13620
V-13621
V-13724
V-13726
V-26326
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-nginx-overlay.xlsx
+++ b/cms-ars-3.1-moderate-nginx-overlay.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-moderate-nginx-stig-overlay/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E9481C-5289-4843-88F0-3F074EA91EF7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D413EB5-E5CD-40F0-AAF1-92A7C4EF356A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="4420" windowWidth="33600" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nginx" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Nginx!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Nginx!$A$1:$H$42</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="231">
   <si>
     <t>Vuln ID</t>
   </si>
@@ -56,51 +56,6 @@
   </si>
   <si>
     <t>NOTES</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CM-6 b</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IA-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AC-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AC-8 a</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SC-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AC-7 a</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AC-7 b</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> AC-6 (10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IA-5 (1) (d)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IA-5 (1) (e)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IA-4 e</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IA-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SC-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SC-8</t>
-  </si>
-  <si>
-    <t>800-53</t>
   </si>
   <si>
     <t>V-2230</t>
@@ -563,15 +518,6 @@
   </si>
   <si>
     <t>Many vulnerabilities are associated with older versions of web server software. As hot fixes and patches are issued, these solutions are included in the next version of the server software. Maintaining the web server at a current version makes the efforts of a malicious user to exploit the web service more difficult.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To determine the version of the nginx software that is running on the system. Use the command:
-nginx -v
-If the version of nginx is not at the following version or higher, this is a finding.
-nginx version: nginx/1.13.0
-Note: In some situations, the nginx software that is being used is supported by another vendor, such as nginx.com. 
-The versions of the software in these cases may not match the above mentioned version numbers. If the site can provide vendor documentation showing the version of the web server is supported, this would not be a finding.
-</t>
   </si>
   <si>
     <t>Install the current version of the web server software and maintain appropriate service packs and patches.</t>
@@ -1147,12 +1093,6 @@
 </t>
   </si>
   <si>
-    <t>Need to configure dmz_subnet attribute</t>
-  </si>
-  <si>
-    <t>need to configure NGINX_MIN_VER</t>
-  </si>
-  <si>
     <t>Obtain a list of the user accounts for the system, noting the privileges for each account.  
 Verify with the system administrator or the ISSO that all privileged accounts are mission essential and documented.
 Verify with the system administrator or the ISSO that all non-administrator access to shell scripts and operating system functions are mission essential and documented.
@@ -1160,15 +1100,6 @@
 If undocumented access to shell scripts or operating system functions is found, this is a finding.</t>
   </si>
   <si>
-    <t>Configure the sys_admin attribute</t>
-  </si>
-  <si>
-    <t>Maybe have to configure email package?</t>
-  </si>
-  <si>
-    <t>Configure monitoring software?</t>
-  </si>
-  <si>
     <t>update to align with changes in simp rhel v-71999
 https://github.cms.gov/ISPG/inspec-profile-disa_stig-el7/blob/78e48ea893b7aa80ea8027b2bc88500d4e2ce89d/controls/V-71999.rb</t>
   </si>
@@ -1229,9 +1160,6 @@
       <t xml:space="preserve">-approved PKIs will be utilized.
 </t>
     </r>
-  </si>
-  <si>
-    <t>Should we just make this a manual check?</t>
   </si>
   <si>
     <r>
@@ -1459,9 +1387,6 @@
     </r>
   </si>
   <si>
-    <t>Should this also be a manual check?</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">The private web server must use an approved </t>
     </r>
@@ -1563,44 +1488,52 @@
     </r>
   </si>
   <si>
-    <t>Left as-is because session lock of 15 minutes doesn't make sense for this.</t>
-  </si>
-  <si>
-    <t>Need to configure to use</t>
-  </si>
-  <si>
-    <t>It looks like we try to do this in an automated way. Should this also be a manual check to review the plans as described in the check field?</t>
-  </si>
-  <si>
-    <t>Make this a manual check that follows new format.</t>
-  </si>
-  <si>
-    <r>
-      <t>Nginx directory and file permissions and ownership should be set per the following table.. The installation directories may vary from one installation to the next.  If used, the WebAmins group should contain only accounts of persons authorized to manage the web server configuration, otherwise the root group should own all Nginx files and directories. 
+    <t>Nginx directory and file permissions and ownership should be set per the following table.. The installation directories may vary from one installation to the next.  If used, the WebAmins group should contain only accounts of persons authorized to manage the web server configuration, otherwise the root group should own all Nginx files and directories. 
 If the files and directories are not set to the following permissions or more restrictive, this is a finding.
 grep for the "root" directive on the nginx.conf file and any separate included configuration files to find the Nginx root directory
 /usr/sbin/nginx        root WebAdmin  550/550
 /etc/nginx/     root WebAdmin 770/660
 /etc/nginx/conf.d     root WebAdmin 770/660
 /etc/nginx/modules    root WebAdmin 770/660
-/usr/share/nginx/html    root WebAdmin  77</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
+/usr/share/nginx/html    root WebAdmin  775/664
+/var/log/nginx       root WebAdmin  750/640
+NOTE:  The permissions are noted as directories / files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use the chmod command to set permissions on the web server system directories and files as follows.
+/usr/sbin/nginx	       root	WebAdmin 	550/550
+/etc/nginx/     root WebAdmin 770/660
+/etc/nginx/conf.d     root WebAdmin 770/660
+/etc/nginx/modules    root WebAdmin 770/660
+/usr/share/nginx/html    root	WebAdmin 	775/664
+/var/log/nginx       root	WebAdmin 	750/640
+</t>
+  </si>
+  <si>
+    <t>describe "For this CMS ARS 3.1 overlay, this control must be reviewed manually" do 
+skip "For this CMS ARS 3.1 overlay, this control must be reviewed manually"
+end</t>
+  </si>
+  <si>
+    <t>User-defined attribute needed to provide the system-specific public DMZ subnet that houses the public web servers. See Readme for this profile.</t>
+  </si>
+  <si>
+    <r>
+      <t>To determine the version of the nginx software that is running on the system. Use the command:
+nginx -v
+If the version of nginx is not at the following version or higher, this is a finding.
+nginx version: nginx/1.1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>0</t>
     </r>
     <r>
       <rPr>
@@ -1610,120 +1543,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/66</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-/var/log/nginx       root WebAdmin  750/640
-NOTE:  The permissions are noted as directories / files</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Use the chmod command to set permissions on the web server system directories and files as follows.
-/usr/sbin/nginx	       root	WebAdmin 	550/550
-/etc/nginx/     root WebAdmin 770/660
-/etc/nginx/conf.d     root WebAdmin 770/660
-/etc/nginx/modules    root WebAdmin 770/660
-/usr/share/nginx/html    root	WebAdmin 	77</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>/66</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-/var/log/nginx       root	WebAdmin 	750/640
-</t>
-    </r>
-  </si>
-  <si>
-    <t>need to configure to work</t>
-  </si>
-  <si>
-    <t>Need to change 775 to prevent public read/write
-Need to change 664 to 660 to prevent public read/write
-need to configure to use</t>
+      <t xml:space="preserve">.0
+Note: In some situations, the nginx software that is being used is supported by another vendor, such as nginx.com. 
+The versions of the software in these cases may not match the above mentioned version numbers. If the site can provide vendor documentation showing the version of the web server is supported, this would not be a finding.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>User-defined attribute needed to provide the specific system administrator, nginx account owner/group   names used for this system. See Readme for this profile.</t>
+  </si>
+  <si>
+    <t>User-defined attribute needed to provide the specific system administrator account name and nginx owner account name used for this system. See Readme for this profile.</t>
+  </si>
+  <si>
+    <t>User-defined attribute(s) needed. See Readme for this profile.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1897,21 +1737,21 @@
       <name val="Calibri (Body)"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="35">
@@ -2295,20 +2135,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2319,7 +2155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2337,22 +2173,25 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2710,31 +2549,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozenSplit"/>
-      <selection activeCell="A2" sqref="A2:B58"/>
-      <selection pane="topRight" activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A59" sqref="A59:XFD339"/>
-      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="7.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="27.83203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="48" style="4" customWidth="1"/>
-    <col min="6" max="6" width="35.1640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="16.1640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="3"/>
-    <col min="10" max="10" width="11" style="3" hidden="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="1" width="8.3125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="7.47265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.20703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="30.26171875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="57.7890625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="28.9453125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.05078125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="8.83984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" customHeight="1">
+    <row r="1" spans="1:8" ht="15.55" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2759,1153 +2596,1019 @@
       <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="331.2">
+      <c r="A2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="230.4">
+      <c r="A3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" ht="316.8">
+      <c r="A4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="158.4">
+      <c r="A5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="273.60000000000002">
+      <c r="A6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="230.4">
+      <c r="A7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="244.8">
+      <c r="A8" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:8" ht="288">
+      <c r="A9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="273.60000000000002">
+      <c r="A10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="360">
+      <c r="A11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="273.60000000000002">
+      <c r="A12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="388.8">
+      <c r="A13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="273.60000000000002">
+      <c r="A14" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="302.39999999999998">
+      <c r="A15" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="230.4">
+      <c r="A16" s="14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="409.6">
-      <c r="A2" s="11" t="s">
+      <c r="B16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" ht="230.4">
+      <c r="A17" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="409.5">
+      <c r="A18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="J2" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="256">
-      <c r="A3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="C18" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="409.5">
+      <c r="A19" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" s="9"/>
-      <c r="J3" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="365">
-      <c r="A4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="C19" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" ht="201.6">
+      <c r="A20" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" ht="409.5">
+      <c r="A21" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="J4" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="208">
-      <c r="A5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="C21" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="331.2">
+      <c r="A22" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="J5" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="320">
-      <c r="A6" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="C22" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="302.39999999999998">
+      <c r="A23" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="302.39999999999998">
+      <c r="A24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="J6" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="272">
-      <c r="A7" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="C24" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" ht="409" customHeight="1">
+      <c r="A25" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" s="15" t="s">
+      <c r="C25" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" ht="244.8">
+      <c r="A26" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" ht="273.60000000000002">
+      <c r="A27" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" ht="201.6">
+      <c r="A28" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" ht="288">
+      <c r="A29" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" ht="244.8">
+      <c r="A30" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" ht="244.8">
+      <c r="A31" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" ht="216">
+      <c r="A32" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" ht="201.6">
+      <c r="A33" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" ht="201.6">
+      <c r="A34" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" ht="129.6">
+      <c r="A35" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" ht="345.6">
+      <c r="A36" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" ht="172.8">
+      <c r="A37" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" ht="331.2">
+      <c r="A38" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H38" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="272">
-      <c r="A8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="335">
-      <c r="A9" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>233</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="320">
-      <c r="A10" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="6" t="s">
+    </row>
+    <row r="39" spans="1:8" ht="187.2">
+      <c r="A39" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="409.6">
-      <c r="A11" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="J11" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="350">
-      <c r="A12" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="C39" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" ht="244.8">
+      <c r="A40" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="J12" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="409.6">
-      <c r="A13" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="C40" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" ht="409" customHeight="1">
+      <c r="A41" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>252</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="335">
-      <c r="A14" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>252</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="365">
-      <c r="A15" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="C41" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" ht="216">
+      <c r="A42" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>253</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="272">
-      <c r="A16" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="256">
-      <c r="A17" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="409.6">
-      <c r="A18" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="409.6">
-      <c r="A19" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="240">
-      <c r="A20" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="J20" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="409.6">
-      <c r="A21" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="409.6">
-      <c r="A22" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>237</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>238</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="365">
-      <c r="A23" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="365">
-      <c r="A24" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="H24" s="9"/>
-      <c r="J24" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="409" customHeight="1">
-      <c r="A25" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="288">
-      <c r="A26" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H26" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="304">
-      <c r="A27" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H27" s="1"/>
-      <c r="J27" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="240">
-      <c r="A28" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H28" s="1"/>
-      <c r="J28" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="320">
-      <c r="A29" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H29" s="1"/>
-      <c r="J29" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="288">
-      <c r="A30" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H30" s="1"/>
-      <c r="J30" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="288">
-      <c r="A31" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H31" s="1"/>
-      <c r="J31" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="256">
-      <c r="A32" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H32" s="1"/>
-      <c r="J32" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="240">
-      <c r="A33" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H33" s="1"/>
-      <c r="J33" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="240">
-      <c r="A34" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H34" s="1"/>
-      <c r="J34" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="144">
-      <c r="A35" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H35" s="1"/>
-      <c r="J35" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="395">
-      <c r="A36" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H36" s="1"/>
-      <c r="J36" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="192">
-      <c r="A37" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="7" t="s">
+      <c r="C42" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H37" s="1"/>
-      <c r="J37" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="395">
-      <c r="A38" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="7" t="s">
+      <c r="E42" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="F42" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E38" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="224">
-      <c r="A39" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="H39" s="1"/>
-      <c r="J39" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="240">
-      <c r="A40" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="H40" s="1"/>
-      <c r="J40" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="409" customHeight="1">
-      <c r="A41" s="16" t="s">
+      <c r="G42" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H41" s="1"/>
-      <c r="J41" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="256">
-      <c r="A42" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="H42" s="1"/>
-      <c r="J42" s="5" t="s">
-        <v>15</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{36045688-EAFA-4F0D-A552-6A9CF4EBD8AA}"/>
+  <autoFilter ref="A1:H42" xr:uid="{24772F0D-3F16-4461-BDCA-C624A095D70F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated based on Eugene's review
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-nginx-overlay.xlsx
+++ b/cms-ars-3.1-moderate-nginx-overlay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-moderate-nginx-stig-overlay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D413EB5-E5CD-40F0-AAF1-92A7C4EF356A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B557C1-D132-0C4D-901E-8D982A3FDF03}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67200" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nginx" sheetId="1" r:id="rId1"/>
@@ -357,32 +357,6 @@
   </si>
   <si>
     <t>Remove any compiler found on the production web server, but if the compiler program is needed to patch or upgrade an application suite in a production environment or the compiler is embedded and will break the suite if removed, document the compiler installation with the ISSO/ISSM and ensure that the compiler is restricted to only administrative users.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A public web server, if hosted on the NIPRNet, must be isolated in an accredited </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">DoD </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DMZ Extension.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1105,30 +1079,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">A private web server’s list of CAs in a trust hierarchy must lead to an authorized  </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">DoD </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PKI Root CA.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">A PKI certificate is a digital identifier that establishes the identity of an individual or a platform. A server that has a certificate provides users with third-party confirmation of authenticity. Most web browsers perform server authentication automatically and the user is notified only if the authentication fails. The authentication process between the server and the client is performed using the SSL/TLS protocol. Digital certificates are authenticated, issued, and managed by a trusted Certificate Authority (CA).
 The use of a trusted certificate validation hierarchy is crucial to the ability to control access to a site’s server and to prevent unauthorized access. Only </t>
     </r>
@@ -1557,6 +1507,93 @@
   </si>
   <si>
     <t>User-defined attribute(s) needed. See Readme for this profile.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A public web server, if hosted on the NIPRNet, must be isolated in an accredited </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">DoD </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">DMZ </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Extension</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A private web server’s list of CAs in a trust hierarchy must lead to an authorized </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CMS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">DoD </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PKI Root CA.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2555,23 +2592,23 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.3125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="7.47265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.20703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="30.26171875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="57.7890625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="28.9453125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.05078125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="8.83984375" style="3"/>
+    <col min="1" max="1" width="8.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="57.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="29" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.55" customHeight="1">
+    <row r="1" spans="1:8" ht="15.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2597,7 +2634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="331.2">
+    <row r="2" spans="1:8" ht="365">
       <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
@@ -2621,7 +2658,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="230.4">
+    <row r="3" spans="1:8" ht="256">
       <c r="A3" s="10" t="s">
         <v>12</v>
       </c>
@@ -2645,7 +2682,7 @@
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" ht="316.8">
+    <row r="4" spans="1:8" ht="335">
       <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
@@ -2669,7 +2706,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="158.4">
+    <row r="5" spans="1:8" ht="176">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -2692,10 +2729,10 @@
         <v>52</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="273.60000000000002">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="304">
       <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
@@ -2703,25 +2740,25 @@
         <v>7</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>54</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="230.4">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="240">
       <c r="A7" s="14" t="s">
         <v>16</v>
       </c>
@@ -2729,25 +2766,25 @@
         <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>54</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="244.8">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="272">
       <c r="A8" s="15" t="s">
         <v>17</v>
       </c>
@@ -2755,23 +2792,23 @@
         <v>8</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="1:8" ht="288">
+    <row r="9" spans="1:8" ht="304">
       <c r="A9" s="14" t="s">
         <v>18</v>
       </c>
@@ -2779,25 +2816,25 @@
         <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>55</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="273.60000000000002">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="304">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
@@ -2805,25 +2842,25 @@
         <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>56</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="360">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="395">
       <c r="A11" s="14" t="s">
         <v>20</v>
       </c>
@@ -2831,23 +2868,23 @@
         <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="273.60000000000002">
+    <row r="12" spans="1:8" ht="304">
       <c r="A12" s="14" t="s">
         <v>21</v>
       </c>
@@ -2855,23 +2892,23 @@
         <v>7</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>57</v>
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="388.8">
+    <row r="13" spans="1:8" ht="409.6">
       <c r="A13" s="14" t="s">
         <v>22</v>
       </c>
@@ -2879,25 +2916,25 @@
         <v>7</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>57</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="273.60000000000002">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="304">
       <c r="A14" s="14" t="s">
         <v>23</v>
       </c>
@@ -2905,25 +2942,25 @@
         <v>9</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="E14" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>115</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>53</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="302.39999999999998">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="320">
       <c r="A15" s="14" t="s">
         <v>24</v>
       </c>
@@ -2931,25 +2968,25 @@
         <v>7</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="E15" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>56</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="230.4">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="256">
       <c r="A16" s="14" t="s">
         <v>25</v>
       </c>
@@ -2957,23 +2994,23 @@
         <v>7</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="E16" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>121</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>52</v>
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="230.4">
+    <row r="17" spans="1:8" ht="240">
       <c r="A17" s="14" t="s">
         <v>26</v>
       </c>
@@ -2981,23 +3018,23 @@
         <v>7</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>125</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>58</v>
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="409.5">
+    <row r="18" spans="1:8" ht="409.6">
       <c r="A18" s="15" t="s">
         <v>27</v>
       </c>
@@ -3005,25 +3042,25 @@
         <v>9</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>59</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="409.5">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="409.6">
       <c r="A19" s="14" t="s">
         <v>28</v>
       </c>
@@ -3031,23 +3068,23 @@
         <v>7</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>133</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>60</v>
       </c>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" ht="201.6">
+    <row r="20" spans="1:8" ht="208">
       <c r="A20" s="14" t="s">
         <v>29</v>
       </c>
@@ -3055,23 +3092,23 @@
         <v>9</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" ht="409.5">
+    <row r="21" spans="1:8" ht="409.6">
       <c r="A21" s="15" t="s">
         <v>30</v>
       </c>
@@ -3079,25 +3116,25 @@
         <v>7</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="E21" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="F21" s="8" t="s">
         <v>140</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>141</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>52</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="331.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="365">
       <c r="A22" s="15" t="s">
         <v>31</v>
       </c>
@@ -3105,25 +3142,25 @@
         <v>7</v>
       </c>
       <c r="C22" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="F22" s="12" t="s">
         <v>217</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>219</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>61</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="302.39999999999998">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="320">
       <c r="A23" s="14" t="s">
         <v>32</v>
       </c>
@@ -3131,25 +3168,25 @@
         <v>8</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="302.39999999999998">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="335">
       <c r="A24" s="15" t="s">
         <v>33</v>
       </c>
@@ -3157,16 +3194,16 @@
         <v>7</v>
       </c>
       <c r="C24" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="F24" s="13" t="s">
         <v>220</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>222</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>61</v>
@@ -3181,23 +3218,23 @@
         <v>7</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" ht="244.8">
+    <row r="26" spans="1:8" ht="272">
       <c r="A26" s="14" t="s">
         <v>35</v>
       </c>
@@ -3205,23 +3242,23 @@
         <v>7</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:8" ht="273.60000000000002">
+    <row r="27" spans="1:8" ht="288">
       <c r="A27" s="14" t="s">
         <v>36</v>
       </c>
@@ -3229,23 +3266,23 @@
         <v>7</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>158</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" ht="201.6">
+    <row r="28" spans="1:8" ht="224">
       <c r="A28" s="14" t="s">
         <v>37</v>
       </c>
@@ -3253,23 +3290,23 @@
         <v>7</v>
       </c>
       <c r="C28" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>162</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" ht="288">
+    <row r="29" spans="1:8" ht="320">
       <c r="A29" s="14" t="s">
         <v>38</v>
       </c>
@@ -3277,23 +3314,23 @@
         <v>7</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>165</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>166</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" ht="244.8">
+    <row r="30" spans="1:8" ht="272">
       <c r="A30" s="14" t="s">
         <v>39</v>
       </c>
@@ -3301,23 +3338,23 @@
         <v>7</v>
       </c>
       <c r="C30" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>169</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>170</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" ht="244.8">
+    <row r="31" spans="1:8" ht="256">
       <c r="A31" s="14" t="s">
         <v>40</v>
       </c>
@@ -3325,23 +3362,23 @@
         <v>7</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="E31" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" ht="216">
+    <row r="32" spans="1:8" ht="240">
       <c r="A32" s="14" t="s">
         <v>41</v>
       </c>
@@ -3349,23 +3386,23 @@
         <v>7</v>
       </c>
       <c r="C32" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="F32" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>178</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>52</v>
       </c>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8" ht="201.6">
+    <row r="33" spans="1:8" ht="208">
       <c r="A33" s="14" t="s">
         <v>42</v>
       </c>
@@ -3373,23 +3410,23 @@
         <v>7</v>
       </c>
       <c r="C33" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="E33" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="F33" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>182</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>62</v>
       </c>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8" ht="201.6">
+    <row r="34" spans="1:8" ht="224">
       <c r="A34" s="14" t="s">
         <v>43</v>
       </c>
@@ -3397,23 +3434,23 @@
         <v>7</v>
       </c>
       <c r="C34" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>185</v>
-      </c>
       <c r="F34" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>57</v>
       </c>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8" ht="129.6">
+    <row r="35" spans="1:8" ht="128">
       <c r="A35" s="14" t="s">
         <v>44</v>
       </c>
@@ -3421,23 +3458,23 @@
         <v>7</v>
       </c>
       <c r="C35" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>188</v>
-      </c>
       <c r="F35" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>57</v>
       </c>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8" ht="345.6">
+    <row r="36" spans="1:8" ht="365">
       <c r="A36" s="14" t="s">
         <v>45</v>
       </c>
@@ -3445,23 +3482,23 @@
         <v>7</v>
       </c>
       <c r="C36" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="E36" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>191</v>
-      </c>
       <c r="F36" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>57</v>
       </c>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:8" ht="172.8">
+    <row r="37" spans="1:8" ht="176">
       <c r="A37" s="14" t="s">
         <v>46</v>
       </c>
@@ -3469,23 +3506,23 @@
         <v>7</v>
       </c>
       <c r="C37" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>195</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>57</v>
       </c>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8" ht="331.2">
+    <row r="38" spans="1:8" ht="365">
       <c r="A38" s="14" t="s">
         <v>47</v>
       </c>
@@ -3493,25 +3530,25 @@
         <v>7</v>
       </c>
       <c r="C38" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="E38" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="F38" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>199</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>64</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="187.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="208">
       <c r="A39" s="14" t="s">
         <v>48</v>
       </c>
@@ -3519,23 +3556,23 @@
         <v>7</v>
       </c>
       <c r="C39" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="E39" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>202</v>
-      </c>
       <c r="F39" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>62</v>
       </c>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:8" ht="244.8">
+    <row r="40" spans="1:8" ht="256">
       <c r="A40" s="14" t="s">
         <v>49</v>
       </c>
@@ -3543,16 +3580,16 @@
         <v>7</v>
       </c>
       <c r="C40" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="E40" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="F40" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>63</v>
@@ -3567,23 +3604,23 @@
         <v>7</v>
       </c>
       <c r="C41" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="E41" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="F41" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>210</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>65</v>
       </c>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:8" ht="216">
+    <row r="42" spans="1:8" ht="240">
       <c r="A42" s="14" t="s">
         <v>51</v>
       </c>
@@ -3591,16 +3628,16 @@
         <v>7</v>
       </c>
       <c r="C42" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="E42" s="5" t="s">
+      <c r="F42" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>213</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>65</v>

</xml_diff>